<commit_message>
ggridge thresholds for poster
</commit_message>
<xml_diff>
--- a/model_thresholds/model_thresholds.xlsx
+++ b/model_thresholds/model_thresholds.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="8_{5D526921-C65C-4DBB-9B54-2604AA2DAF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC044C8-D985-4EE5-B6FA-0F6B9AA595EC}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="7200" windowWidth="29040" windowHeight="16440" xr2:uid="{757F9C19-9E94-4D92-AB18-7EEE77F93D94}"/>
+    <workbookView xWindow="-28920" yWindow="-2040" windowWidth="29040" windowHeight="15720" xr2:uid="{757F9C19-9E94-4D92-AB18-7EEE77F93D94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,17 +426,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -458,7 +458,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -469,7 +469,7 @@
         <v>0.46300000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -480,7 +480,7 @@
         <v>0.36799999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0.85099999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -502,7 +502,7 @@
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>

</xml_diff>